<commit_message>
Updated Layout and BOM
Found some mismatches in the BOM and added the fixes.  Also, updated
Layout to use the files with the corrected silkscreen.
</commit_message>
<xml_diff>
--- a/Design Files/Schematic-BOM/BD9G101G-EVK-101_BOM_10-22-2015.xlsx
+++ b/Design Files/Schematic-BOM/BD9G101G-EVK-101_BOM_10-22-2015.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>BOM for BD9G101G</t>
   </si>
@@ -104,9 +104,6 @@
     <t>5V, 0.5A</t>
   </si>
   <si>
-    <t>BDG101G</t>
-  </si>
-  <si>
     <t>SSOP6</t>
   </si>
   <si>
@@ -189,12 +186,60 @@
   </si>
   <si>
     <t xml:space="preserve">Black Test Pin </t>
+  </si>
+  <si>
+    <t>JEN</t>
+  </si>
+  <si>
+    <t>RFRA</t>
+  </si>
+  <si>
+    <t>RFB</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>36-5005-ND</t>
+  </si>
+  <si>
+    <t>36-5006-ND</t>
+  </si>
+  <si>
+    <t>Keystone</t>
+  </si>
+  <si>
+    <t>Via</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>RHM0.0CGTR-ND</t>
+  </si>
+  <si>
+    <t>MCR03ERTJ000</t>
+  </si>
+  <si>
+    <t>SMAJ30ALFCT-ND</t>
+  </si>
+  <si>
+    <t>BD9G101G</t>
+  </si>
+  <si>
+    <t>BD9G101G-CT-ND</t>
+  </si>
+  <si>
+    <t>490-14207-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -449,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -495,6 +540,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -502,15 +559,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -607,6 +655,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -642,6 +707,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -818,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,36 +916,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="23" t="s">
         <v>13</v>
       </c>
     </row>
@@ -872,7 +954,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>25</v>
@@ -884,13 +966,13 @@
         <v>16</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>23</v>
@@ -902,16 +984,16 @@
         <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
@@ -923,10 +1005,10 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -935,19 +1017,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" s="10"/>
     </row>
@@ -959,16 +1041,16 @@
         <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="G7" s="10"/>
     </row>
@@ -980,16 +1062,16 @@
         <v>10</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" s="10"/>
     </row>
@@ -1009,7 +1091,9 @@
       <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1020,59 +1104,144 @@
         <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="F15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="B16" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="16"/>
+      <c r="F16" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>